<commit_message>
Final submission accepted in Frontiers in Cardiovascular Medicine
</commit_message>
<xml_diff>
--- a/GridSearchCV_results/interpretability_metrics.xlsx
+++ b/GridSearchCV_results/interpretability_metrics.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k5000751\OneDrive - Epedu O365\SeAMK\GitHub\Heart_Failure_Predictor\GridSearchCV_results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tuni-my.sharepoint.com/personal/pedro_morenosanchez_tuni_fi/Documents/Documents/GitHub/Heart_Failure_Predictor/GridSearchCV_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{9D1ECF4F-B7A6-4B3D-9220-FCA701796014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{54360B42-6AAE-4A0E-9F52-434EE998EAD4}"/>
+  <xr:revisionPtr revIDLastSave="118" documentId="8_{9D1ECF4F-B7A6-4B3D-9220-FCA701796014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{066F18C0-9F62-4AE4-84BD-01DD2A20DBD2}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7590" xr2:uid="{417D218A-D2DC-4700-82DF-E7205B1FAA64}"/>
+    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" activeTab="1" xr2:uid="{417D218A-D2DC-4700-82DF-E7205B1FAA64}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RF" sheetId="1" r:id="rId1"/>
+    <sheet name="ET" sheetId="5" r:id="rId2"/>
+    <sheet name="AB" sheetId="4" r:id="rId3"/>
+    <sheet name="GB" sheetId="3" r:id="rId4"/>
+    <sheet name="XGB" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="11">
   <si>
     <t>Rationale: For interpretability metrics we will take the DT as a fully interpretable model and then compare them with our best estimator.</t>
   </si>
@@ -456,23 +460,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B46D28C-966F-4413-BD8A-E4FFA052E783}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.08984375" customWidth="1"/>
-    <col min="2" max="2" width="17.7265625" customWidth="1"/>
-    <col min="3" max="3" width="16.36328125" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>6</v>
       </c>
@@ -486,7 +490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -494,17 +498,17 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="1">
         <f>B4/C4</f>
-        <v>0.66666666666666663</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -512,31 +516,38 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2">
-        <v>0.67777777777777781</v>
+        <v>0.75</v>
       </c>
       <c r="C6">
-        <v>0.83333333333333337</v>
+        <v>0.74</v>
       </c>
       <c r="D6" s="1">
         <f>B6/C6</f>
-        <v>0.81333333333333335</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1.0135135135135136</v>
+      </c>
+      <c r="E6">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="3">
         <f>D6/(D6+D4)</f>
-        <v>0.5495495495495496</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0.58221594918842623</v>
+      </c>
+      <c r="E8" s="3">
+        <f>E6/(E6+D4)</f>
+        <v>0.57649550026469032</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
@@ -544,7 +555,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>2</v>
       </c>
@@ -552,7 +563,7 @@
         <v>0.81</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -566,7 +577,505 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499F0EC3-F831-4BE9-8259-8C89BA5F318E}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(B4)/C4</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="C6">
+        <v>0.83</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v>0.9783132530120483</v>
+      </c>
+      <c r="E6">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <f>D6/(D6+D4)</f>
+        <v>0.64203565267395069</v>
+      </c>
+      <c r="E8" s="3">
+        <f>E6/(E6+D4)</f>
+        <v>0.63280293757649941</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D6999D-F878-4774-8EBA-3BB3459E0573}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(C4-B4)/C4</f>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="C6">
+        <v>0.76</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v>1.0684210526315789</v>
+      </c>
+      <c r="E6">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <f>D6/(D6+D4)</f>
+        <v>0.64684014869888473</v>
+      </c>
+      <c r="E8" s="3">
+        <f>E6/(E6+D4)</f>
+        <v>0.62923728813559321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8781562B-EE69-490A-8C5C-5CEEA4BE40D4}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(C4-B4)/C4</f>
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="C6">
+        <v>0.74</v>
+      </c>
+      <c r="D6" s="1">
+        <f>B6/C6</f>
+        <v>1.027027027027027</v>
+      </c>
+      <c r="E6">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <f>D6/(D6+D4)</f>
+        <v>0.7113884555382215</v>
+      </c>
+      <c r="E8" s="3">
+        <f>E6/(E6+D4)</f>
+        <v>0.70379146919431279</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1293B76D-BB2E-408F-9361-5B992DB60359}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1">
+        <f>(C4-B4)/C4</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="C6">
+        <v>0.75</v>
+      </c>
+      <c r="D6" s="1">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="E6">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="3">
+        <f>D6/(D6+D4)</f>
+        <v>2.8843352432747403E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <f>E6/(E6+D4)</f>
+        <v>0.74811083123425692</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Asiakirja" ma:contentTypeID="0x01010023A5052220506F469AB01ED2533FD06A" ma:contentTypeVersion="9" ma:contentTypeDescription="Luo uusi asiakirja." ma:contentTypeScope="" ma:versionID="fd68578c2226425a2e97903507939f58">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1c94d993-416a-4bc5-a0c8-faa13ae8012f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30fd0e0c1b4e0ef2d317b66ad0932bf0" ns3:_="">
     <xsd:import namespace="1c94d993-416a-4bc5-a0c8-faa13ae8012f"/>
@@ -744,22 +1253,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4656D8-8CB7-4DC0-A603-1FCA793B1B39}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7854A29-7C9A-4DDB-AE32-3463A5E82648}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BE0A1E9-8516-4823-A65A-4747D670F9F2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -775,21 +1286,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B7854A29-7C9A-4DDB-AE32-3463A5E82648}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B4656D8-8CB7-4DC0-A603-1FCA793B1B39}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>